<commit_message>
analyzed a few more programs
</commit_message>
<xml_diff>
--- a/kodu_programs.xlsx
+++ b/kodu_programs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="13320" windowWidth="20980" windowHeight="15040"/>
+    <workbookView xWindow="-28800" yWindow="12540" windowWidth="28800" windowHeight="17480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="122">
   <si>
     <t>No-op</t>
   </si>
@@ -319,6 +319,78 @@
   </si>
   <si>
     <t xml:space="preserve"> HCIactors</t>
+  </si>
+  <si>
+    <t>feature envy</t>
+  </si>
+  <si>
+    <t>cloud2 watches scorebucket yellow nut other characters modify it</t>
+  </si>
+  <si>
+    <t>unused field</t>
+  </si>
+  <si>
+    <t>scorebucket.color.red is written to but never read</t>
+  </si>
+  <si>
+    <t>Need to determine smelly threshold!</t>
+  </si>
+  <si>
+    <t>duplicate code</t>
+  </si>
+  <si>
+    <t>fish1 has two identical 'when' clauses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cloud1 </t>
+  </si>
+  <si>
+    <t>has  identical when clauses</t>
+  </si>
+  <si>
+    <t>kodu1</t>
+  </si>
+  <si>
+    <t>jet1</t>
+  </si>
+  <si>
+    <t>sub1</t>
+  </si>
+  <si>
+    <t>cycle1</t>
+  </si>
+  <si>
+    <t>balloon2</t>
+  </si>
+  <si>
+    <t>long method</t>
+  </si>
+  <si>
+    <t>kodu2</t>
+  </si>
+  <si>
+    <t>has 9 rules</t>
+  </si>
+  <si>
+    <t>has 10 rules</t>
+  </si>
+  <si>
+    <t>30 characters hace identical when clauses</t>
+  </si>
+  <si>
+    <t>has identical when clauses</t>
+  </si>
+  <si>
+    <t>lazy class</t>
+  </si>
+  <si>
+    <t>factory 1</t>
+  </si>
+  <si>
+    <t>has 7 rules</t>
+  </si>
+  <si>
+    <t>has 6 rules</t>
   </si>
 </sst>
 </file>
@@ -390,14 +462,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -410,12 +496,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -694,9 +795,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF30"/>
+  <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -818,10 +919,34 @@
       <c r="B3" t="s">
         <v>92</v>
       </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="F3">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
       </c>
       <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
         <v>0</v>
       </c>
     </row>
@@ -832,10 +957,34 @@
       <c r="B4" t="s">
         <v>36</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="F4">
         <v>12</v>
       </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
       <c r="H4" s="7">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>0</v>
       </c>
     </row>
@@ -846,26 +995,45 @@
       <c r="B5" t="s">
         <v>38</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <v>2</v>
       </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
       <c r="H5" s="7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:32">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" hidden="1">
       <c r="A6" t="s">
         <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7">
-        <v>0</v>
-      </c>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:32">
       <c r="A7" t="s">
@@ -874,10 +1042,34 @@
       <c r="B7" t="s">
         <v>42</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
       <c r="F7">
         <v>45</v>
       </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
       <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
         <v>0</v>
       </c>
     </row>
@@ -888,11 +1080,35 @@
       <c r="B8" t="s">
         <v>44</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
       <c r="F8">
         <v>13</v>
       </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
       <c r="H8" s="7">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:32">
@@ -902,11 +1118,20 @@
       <c r="B9" t="s">
         <v>46</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="F9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H9" s="7">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:32">
@@ -916,12 +1141,7 @@
       <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="F10">
-        <v>8</v>
-      </c>
-      <c r="H10" s="7">
-        <v>0</v>
-      </c>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:32">
       <c r="A11" t="s">
@@ -930,12 +1150,7 @@
       <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="F11">
-        <v>16</v>
-      </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:32">
       <c r="A12" s="6" t="s">
@@ -944,12 +1159,7 @@
       <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="7">
-        <v>1</v>
-      </c>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:32">
       <c r="A13" s="6" t="s">
@@ -958,12 +1168,7 @@
       <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="7">
-        <v>2</v>
-      </c>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:32">
       <c r="A14" t="s">
@@ -972,12 +1177,7 @@
       <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="F14">
-        <v>13</v>
-      </c>
-      <c r="H14" s="7">
-        <v>1</v>
-      </c>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:32">
       <c r="A15" t="s">
@@ -986,12 +1186,7 @@
       <c r="B15" t="s">
         <v>58</v>
       </c>
-      <c r="F15">
-        <v>41</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0</v>
-      </c>
+      <c r="H15" s="7"/>
     </row>
     <row r="16" spans="1:32">
       <c r="A16" t="s">
@@ -1000,12 +1195,7 @@
       <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="F16">
-        <v>25</v>
-      </c>
-      <c r="H16" s="7">
-        <v>0</v>
-      </c>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
@@ -1014,12 +1204,7 @@
       <c r="B17" t="s">
         <v>62</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="H17" s="7">
-        <v>2</v>
-      </c>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
@@ -1028,12 +1213,7 @@
       <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="F18">
-        <v>9</v>
-      </c>
-      <c r="H18" s="7">
-        <v>0</v>
-      </c>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
@@ -1042,12 +1222,7 @@
       <c r="B19" t="s">
         <v>66</v>
       </c>
-      <c r="F19">
-        <v>20</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0</v>
-      </c>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
@@ -1057,12 +1232,7 @@
         <v>68</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="F20">
-        <v>7</v>
-      </c>
-      <c r="H20" s="7">
-        <v>1</v>
-      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
@@ -1071,12 +1241,7 @@
       <c r="B21" t="s">
         <v>70</v>
       </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="H21" s="7">
-        <v>1</v>
-      </c>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
@@ -1085,12 +1250,7 @@
       <c r="B22" t="s">
         <v>72</v>
       </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="H22" s="7">
-        <v>0</v>
-      </c>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
@@ -1099,12 +1259,7 @@
       <c r="B23" t="s">
         <v>74</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="H23" s="7">
-        <v>3</v>
-      </c>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
@@ -1113,12 +1268,7 @@
       <c r="B24" t="s">
         <v>76</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="H24" s="7">
-        <v>1</v>
-      </c>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
@@ -1127,12 +1277,7 @@
       <c r="B25" t="s">
         <v>78</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="H25" s="7">
-        <v>0</v>
-      </c>
+      <c r="H25" s="7"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
@@ -1141,12 +1286,7 @@
       <c r="B26" t="s">
         <v>80</v>
       </c>
-      <c r="F26">
-        <v>19</v>
-      </c>
-      <c r="H26" s="7">
-        <v>0</v>
-      </c>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
@@ -1155,12 +1295,7 @@
       <c r="B27" t="s">
         <v>82</v>
       </c>
-      <c r="F27">
-        <v>2</v>
-      </c>
-      <c r="H27" s="7">
-        <v>6</v>
-      </c>
+      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
@@ -1169,12 +1304,7 @@
       <c r="B28" t="s">
         <v>84</v>
       </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="H28" s="7">
-        <v>0</v>
-      </c>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
@@ -1183,12 +1313,7 @@
       <c r="B29" t="s">
         <v>86</v>
       </c>
-      <c r="F29">
-        <v>58</v>
-      </c>
-      <c r="H29" s="7">
-        <v>7</v>
-      </c>
+      <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
@@ -1197,11 +1322,11 @@
       <c r="B30" t="s">
         <v>88</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="H30" s="7">
-        <v>2</v>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="35" spans="8:8">
+      <c r="H35" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1220,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -1232,7 +1357,7 @@
     <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1243,14 +1368,172 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="5" customFormat="1"/>
-    <row r="4" spans="1:3">
-      <c r="C4" s="4"/>
-    </row>
-    <row r="22" s="5" customFormat="1"/>
-    <row r="31" s="5" customFormat="1"/>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="5" customFormat="1">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="C6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="C7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="B16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" s="5" customFormat="1"/>
+    <row r="32" spans="2:4" s="5" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1264,7 +1547,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -1354,6 +1637,9 @@
       <c r="F4">
         <v>42</v>
       </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
@@ -1374,8 +1660,11 @@
       <c r="F5">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" hidden="1">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1414,6 +1703,9 @@
       <c r="F7">
         <v>7</v>
       </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
@@ -1434,6 +1726,9 @@
       <c r="F8">
         <v>10</v>
       </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
@@ -1454,6 +1749,9 @@
       <c r="F9">
         <v>26</v>
       </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
@@ -1877,6 +2175,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
looked for smells in 17 Kodu programs
</commit_message>
<xml_diff>
--- a/kodu_programs.xlsx
+++ b/kodu_programs.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="145">
   <si>
     <t>No-op</t>
   </si>
@@ -391,6 +391,75 @@
   </si>
   <si>
     <t>has 6 rules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">saucer1 </t>
+  </si>
+  <si>
+    <t>has 5 rules</t>
+  </si>
+  <si>
+    <t>push pad 1</t>
+  </si>
+  <si>
+    <t>balloon1</t>
+  </si>
+  <si>
+    <t>sputnik 1</t>
+  </si>
+  <si>
+    <t>mine1</t>
+  </si>
+  <si>
+    <t>cannon1</t>
+  </si>
+  <si>
+    <t>saucer1has 5 rules</t>
+  </si>
+  <si>
+    <t>reads a score but never writes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kodu1 </t>
+  </si>
+  <si>
+    <t>has 13 rules</t>
+  </si>
+  <si>
+    <t>score is written, not read</t>
+  </si>
+  <si>
+    <t>cannon4</t>
+  </si>
+  <si>
+    <t>sputnik3</t>
+  </si>
+  <si>
+    <t>dead code</t>
+  </si>
+  <si>
+    <t>cannon 12</t>
+  </si>
+  <si>
+    <t>has 6, 8 rules</t>
+  </si>
+  <si>
+    <t>kodu3</t>
+  </si>
+  <si>
+    <t>red scorebucket written not read</t>
+  </si>
+  <si>
+    <t>saucer1</t>
+  </si>
+  <si>
+    <t>inappropriate intimacy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 balloons only check the status of the red and white fastbots </t>
+  </si>
+  <si>
+    <t>cycle2</t>
   </si>
 </sst>
 </file>
@@ -462,7 +531,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -482,8 +551,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -497,8 +586,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -508,6 +598,16 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -517,6 +617,16 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -798,7 +908,7 @@
   <dimension ref="A1:AF35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -947,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:32">
@@ -1121,17 +1231,32 @@
       <c r="C9">
         <v>0</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
       <c r="H9" s="7">
         <v>0</v>
       </c>
       <c r="I9">
         <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:32">
@@ -1141,7 +1266,36 @@
       <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:32">
       <c r="A11" t="s">
@@ -1150,7 +1304,36 @@
       <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>16</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>4</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:32">
       <c r="A12" s="6" t="s">
@@ -1159,7 +1342,36 @@
       <c r="B12" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>107</v>
+      </c>
     </row>
     <row r="13" spans="1:32">
       <c r="A13" s="6" t="s">
@@ -1168,7 +1380,36 @@
       <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="7"/>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:32">
       <c r="A14" t="s">
@@ -1177,7 +1418,36 @@
       <c r="B14" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="7"/>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:32">
       <c r="A15" t="s">
@@ -1186,7 +1456,36 @@
       <c r="B15" t="s">
         <v>58</v>
       </c>
-      <c r="H15" s="7"/>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>51</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="7">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:32">
       <c r="A16" t="s">
@@ -1195,36 +1494,135 @@
       <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>29</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7">
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>61</v>
       </c>
       <c r="B17" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>63</v>
       </c>
       <c r="B18" t="s">
         <v>64</v>
       </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>65</v>
       </c>
       <c r="B19" t="s">
         <v>66</v>
       </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>21</v>
+      </c>
       <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1234,7 +1632,7 @@
       <c r="D20" s="1"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1243,7 +1641,7 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -1252,7 +1650,7 @@
       </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1261,7 +1659,7 @@
       </c>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -1270,7 +1668,7 @@
       </c>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -1279,7 +1677,7 @@
       </c>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1288,7 +1686,7 @@
       </c>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -1297,7 +1695,7 @@
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -1306,7 +1704,7 @@
       </c>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -1315,7 +1713,7 @@
       </c>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>87</v>
       </c>
@@ -1345,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="B2:C2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -1518,7 +1916,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="1:4">
       <c r="B17" t="s">
         <v>112</v>
       </c>
@@ -1529,8 +1927,234 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="2:4" s="5" customFormat="1"/>
-    <row r="32" spans="2:4" s="5" customFormat="1"/>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>112</v>
+      </c>
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D18" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="C20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>103</v>
+      </c>
+      <c r="C21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="C22" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="5" customFormat="1">
+      <c r="C23" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="C24" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="B29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="B30" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="5" customFormat="1">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="B33" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="C35" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="B37" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="C41" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1546,8 +2170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
@@ -1772,6 +2396,9 @@
       <c r="F10">
         <v>19</v>
       </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
@@ -1792,6 +2419,9 @@
       <c r="F11">
         <v>18</v>
       </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
@@ -1812,6 +2442,9 @@
       <c r="F12">
         <v>60</v>
       </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
@@ -1832,6 +2465,9 @@
       <c r="F13">
         <v>47</v>
       </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
@@ -1852,6 +2488,9 @@
       <c r="F14">
         <v>6</v>
       </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
@@ -1872,6 +2511,9 @@
       <c r="F15">
         <v>22</v>
       </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
@@ -1892,8 +2534,11 @@
       <c r="F16">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -1912,8 +2557,11 @@
       <c r="F17">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1932,8 +2580,11 @@
       <c r="F18">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -1952,8 +2603,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -1973,7 +2627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>69</v>
       </c>
@@ -1993,7 +2647,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -2013,7 +2667,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -2033,7 +2687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -2053,7 +2707,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -2073,7 +2727,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -2093,7 +2747,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -2113,7 +2767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -2133,7 +2787,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>85</v>
       </c>
@@ -2153,7 +2807,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
modified the metadata about the kodu programs
</commit_message>
<xml_diff>
--- a/kodu_programs.xlsx
+++ b/kodu_programs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="28760" windowHeight="17480"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="16580" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="548">
   <si>
     <t>No-op</t>
   </si>
@@ -1660,6 +1660,15 @@
   </si>
   <si>
     <t>coin 1</t>
+  </si>
+  <si>
+    <t>Actors</t>
+  </si>
+  <si>
+    <t>Smells</t>
+  </si>
+  <si>
+    <t>HCI</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1722,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1728,6 +1737,17 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1811,7 +1831,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1836,14 +1856,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2194,9 +2215,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
   <cols>
@@ -2252,6 +2271,9 @@
       </c>
       <c r="M1" t="s">
         <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>546</v>
       </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
@@ -4511,15 +4533,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:14">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -4539,7 +4561,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1">
+    <row r="2" spans="1:14" s="5" customFormat="1">
       <c r="A2" s="10" t="s">
         <v>345</v>
       </c>
@@ -4559,10 +4581,10 @@
         <v>439</v>
       </c>
       <c r="G2" s="5">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="14" customFormat="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="14" customFormat="1">
       <c r="A3" s="13" t="s">
         <v>358</v>
       </c>
@@ -4582,10 +4604,10 @@
         <v>280</v>
       </c>
       <c r="G3" s="14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="14" customFormat="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="14" customFormat="1">
       <c r="A4" s="13" t="s">
         <v>199</v>
       </c>
@@ -4607,8 +4629,23 @@
       <c r="G4" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" s="14" customFormat="1">
+      <c r="J4" t="s">
+        <v>545</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>523</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>524</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="14" customFormat="1">
       <c r="A5" s="13" t="s">
         <v>498</v>
       </c>
@@ -4630,8 +4667,31 @@
       <c r="G5" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" s="14" customFormat="1">
+      <c r="I5" s="14" t="s">
+        <v>546</v>
+      </c>
+      <c r="J5" s="5">
+        <f>CORREL(C2:C29, Overview!N2:N29)</f>
+        <v>0.43913030963959626</v>
+      </c>
+      <c r="K5" s="14">
+        <f>CORREL(D2:D29, Overview!N2:N29)</f>
+        <v>0.47063173876900355</v>
+      </c>
+      <c r="L5" s="14">
+        <f>CORREL(E2:E29, Overview!N2:N29)</f>
+        <v>0.56739809209788483</v>
+      </c>
+      <c r="M5" s="14">
+        <f>CORREL(F2:F29, Overview!N2:N29)</f>
+        <v>0.55191808200486869</v>
+      </c>
+      <c r="N5" s="14">
+        <f>CORREL(G2:G29, Overview!N2:N29)</f>
+        <v>0.38403886886909833</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="14" customFormat="1">
       <c r="A6" s="13" t="s">
         <v>168</v>
       </c>
@@ -4654,7 +4714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="14" customFormat="1">
+    <row r="7" spans="1:14" s="14" customFormat="1">
       <c r="A7" s="15" t="s">
         <v>400</v>
       </c>
@@ -4674,10 +4734,10 @@
         <v>118</v>
       </c>
       <c r="G7" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="14" customFormat="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="14" customFormat="1">
       <c r="A8" s="15" t="s">
         <v>209</v>
       </c>
@@ -4697,10 +4757,10 @@
         <v>537</v>
       </c>
       <c r="G8" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="14" customFormat="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="14" customFormat="1">
       <c r="A9" s="13" t="s">
         <v>442</v>
       </c>
@@ -4723,7 +4783,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="14" customFormat="1">
+    <row r="10" spans="1:14" s="14" customFormat="1">
       <c r="A10" s="13" t="s">
         <v>391</v>
       </c>
@@ -4746,7 +4806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="17" customFormat="1" ht="26" thickBot="1">
+    <row r="11" spans="1:14" s="17" customFormat="1" ht="26" thickBot="1">
       <c r="A11" s="16" t="s">
         <v>505</v>
       </c>
@@ -4769,7 +4829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:14">
       <c r="A12" s="14" t="s">
         <v>67</v>
       </c>
@@ -4789,10 +4849,10 @@
         <v>90</v>
       </c>
       <c r="G12" s="14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -4812,10 +4872,10 @@
         <v>64</v>
       </c>
       <c r="G13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -4835,10 +4895,10 @@
         <v>252</v>
       </c>
       <c r="G14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -4858,10 +4918,10 @@
         <v>150</v>
       </c>
       <c r="G15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" hidden="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" hidden="1">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -4904,7 +4964,7 @@
         <v>121</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -4927,7 +4987,7 @@
         <v>418</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -4950,7 +5010,7 @@
         <v>535</v>
       </c>
       <c r="G19">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -4973,7 +5033,7 @@
         <v>141</v>
       </c>
       <c r="G20">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -4996,7 +5056,7 @@
         <v>66</v>
       </c>
       <c r="G21" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -5019,7 +5079,7 @@
         <v>227</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -5042,7 +5102,7 @@
         <v>230</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -5065,7 +5125,7 @@
         <v>244</v>
       </c>
       <c r="G24">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -5088,7 +5148,7 @@
         <v>81</v>
       </c>
       <c r="G25">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -5134,7 +5194,7 @@
         <v>54</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -5157,30 +5217,30 @@
         <v>90</v>
       </c>
       <c r="G28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" s="20" customFormat="1" ht="26" thickBot="1">
+      <c r="A29" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="20">
         <v>28</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="20">
         <v>7</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="20">
         <v>23</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="20">
         <v>103</v>
       </c>
-      <c r="G29">
-        <v>3</v>
+      <c r="G29" s="20">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -5203,7 +5263,7 @@
         <v>267</v>
       </c>
       <c r="G30">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -5226,7 +5286,7 @@
         <v>257</v>
       </c>
       <c r="G31">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -5249,7 +5309,7 @@
         <v>118</v>
       </c>
       <c r="G32">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -5272,7 +5332,7 @@
         <v>186</v>
       </c>
       <c r="G33">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -5295,7 +5355,7 @@
         <v>10</v>
       </c>
       <c r="G34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -5318,7 +5378,7 @@
         <v>550</v>
       </c>
       <c r="G35">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -5341,7 +5401,7 @@
         <v>200</v>
       </c>
       <c r="G36">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -5364,7 +5424,7 @@
         <v>168</v>
       </c>
       <c r="G37">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -5410,7 +5470,7 @@
         <v>122</v>
       </c>
       <c r="G39">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 10 programs from Kodu community
</commit_message>
<xml_diff>
--- a/kodu_programs.xlsx
+++ b/kodu_programs.xlsx
@@ -2215,7 +2215,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
   <cols>
@@ -2662,7 +2664,10 @@
         <v>1</v>
       </c>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="P7" s="2">
+        <f>AVERAGE(N2:N11)</f>
+        <v>3.9</v>
+      </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -2726,7 +2731,10 @@
         <v>8</v>
       </c>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="P8" s="2">
+        <f>AVERAGE(N12:N29)</f>
+        <v>2.5555555555555554</v>
+      </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>

</xml_diff>

<commit_message>
small changes to spreadsheets
</commit_message>
<xml_diff>
--- a/kodu_programs.xlsx
+++ b/kodu_programs.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kstolee/Documents/Research-git/end_user_refactoring/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="16580" windowHeight="17480"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="16580" windowHeight="14820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="Blocks per Program" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -2205,7 +2210,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2215,28 +2220,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView topLeftCell="A6" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.59765625" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.81640625" customWidth="1"/>
-    <col min="3" max="3" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.796875" customWidth="1"/>
+    <col min="3" max="3" width="4.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.19921875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="54" customHeight="1">
+    <row r="1" spans="1:33" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2297,7 +2302,7 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="3"/>
     </row>
-    <row r="2" spans="1:33" s="5" customFormat="1" ht="27" customHeight="1">
+    <row r="2" spans="1:33" s="5" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>345</v>
       </c>
@@ -2323,7 +2328,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="5">
         <v>17</v>
@@ -2339,7 +2344,7 @@
       </c>
       <c r="N2">
         <f>COUNTIF(D2:M2, "&gt;0")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O2" s="11"/>
       <c r="P2" s="11"/>
@@ -2361,7 +2366,7 @@
       <c r="AF2" s="11"/>
       <c r="AG2" s="12"/>
     </row>
-    <row r="3" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1">
+    <row r="3" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>358</v>
       </c>
@@ -2387,7 +2392,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J3" s="14">
         <v>9</v>
@@ -2402,8 +2407,8 @@
         <v>2</v>
       </c>
       <c r="N3">
-        <f>COUNTIF(D3:M3, "&gt;0")</f>
-        <v>5</v>
+        <f t="shared" ref="N2:N12" si="0">COUNTIF(D3:M3, "&gt;0")</f>
+        <v>4</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>150</v>
@@ -2427,7 +2432,7 @@
       <c r="AF3" s="2"/>
       <c r="AG3" s="3"/>
     </row>
-    <row r="4" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1">
+    <row r="4" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>199</v>
       </c>
@@ -2468,7 +2473,7 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <f>COUNTIF(D4:M4, "&gt;0")</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="O4" s="2"/>
@@ -2491,7 +2496,7 @@
       <c r="AF4" s="2"/>
       <c r="AG4" s="3"/>
     </row>
-    <row r="5" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1">
+    <row r="5" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>498</v>
       </c>
@@ -2532,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <f>COUNTIF(D5:M5, "&gt;0")</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="O5" s="2"/>
@@ -2555,7 +2560,7 @@
       <c r="AF5" s="2"/>
       <c r="AG5" s="3"/>
     </row>
-    <row r="6" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1">
+    <row r="6" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>168</v>
       </c>
@@ -2596,7 +2601,7 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <f>COUNTIF(D6:M6, "&gt;0")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O6" s="2"/>
@@ -2619,7 +2624,7 @@
       <c r="AF6" s="2"/>
       <c r="AG6" s="3"/>
     </row>
-    <row r="7" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1">
+    <row r="7" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>400</v>
       </c>
@@ -2660,13 +2665,13 @@
         <v>0</v>
       </c>
       <c r="N7">
-        <f>COUNTIF(D7:M7, "&gt;0")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2">
         <f>AVERAGE(N2:N11)</f>
-        <v>3.9</v>
+        <v>3.5</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -2686,7 +2691,7 @@
       <c r="AF7" s="2"/>
       <c r="AG7" s="3"/>
     </row>
-    <row r="8" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1">
+    <row r="8" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>209</v>
       </c>
@@ -2712,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J8" s="14">
         <v>16</v>
@@ -2727,13 +2732,13 @@
         <v>1</v>
       </c>
       <c r="N8">
-        <f>COUNTIF(D8:M8, "&gt;0")</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2">
         <f>AVERAGE(N12:N29)</f>
-        <v>2.5555555555555554</v>
+        <v>2.2777777777777777</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -2753,7 +2758,7 @@
       <c r="AF8" s="2"/>
       <c r="AG8" s="3"/>
     </row>
-    <row r="9" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1">
+    <row r="9" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>442</v>
       </c>
@@ -2779,7 +2784,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="14">
         <v>16</v>
@@ -2794,8 +2799,8 @@
         <v>43</v>
       </c>
       <c r="N9">
-        <f>COUNTIF(D9:M9, "&gt;0")</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
@@ -2817,7 +2822,7 @@
       <c r="AF9" s="2"/>
       <c r="AG9" s="3"/>
     </row>
-    <row r="10" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1">
+    <row r="10" spans="1:33" s="14" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>391</v>
       </c>
@@ -2858,7 +2863,7 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <f>COUNTIF(D10:M10, "&gt;0")</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O10" s="2"/>
@@ -2881,7 +2886,7 @@
       <c r="AF10" s="2"/>
       <c r="AG10" s="3"/>
     </row>
-    <row r="11" spans="1:33" s="17" customFormat="1" ht="27" customHeight="1" thickBot="1">
+    <row r="11" spans="1:33" s="17" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>505</v>
       </c>
@@ -2907,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J11" s="17">
         <v>116</v>
@@ -2922,7 +2927,7 @@
         <v>56</v>
       </c>
       <c r="N11">
-        <f>COUNTIF(D11:M11, "&gt;0")</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="O11" s="18"/>
@@ -2945,7 +2950,7 @@
       <c r="AF11" s="18"/>
       <c r="AG11" s="19"/>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2986,11 +2991,11 @@
         <v>0</v>
       </c>
       <c r="N12">
-        <f>COUNTIF(D12:M12, "&gt;0")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:33">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -3016,7 +3021,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -3031,11 +3036,11 @@
         <v>1</v>
       </c>
       <c r="N13">
-        <f t="shared" ref="N13:N29" si="0">COUNTIF(D13:M13, "&gt;0")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:33">
+        <f t="shared" ref="N13:N29" si="1">COUNTIF(D13:M13, "&gt;0")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3061,7 +3066,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J14">
         <v>7</v>
@@ -3076,11 +3081,11 @@
         <v>0</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:33">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -3121,11 +3126,11 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:33" hidden="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -3148,11 +3153,11 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -3193,11 +3198,11 @@
         <v>0</v>
       </c>
       <c r="N17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -3223,7 +3228,7 @@
         <v>0</v>
       </c>
       <c r="I18" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>32</v>
@@ -3238,11 +3243,11 @@
         <v>0</v>
       </c>
       <c r="N18">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -3283,11 +3288,11 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -3328,11 +3333,11 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -3358,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <v>4</v>
@@ -3373,11 +3378,11 @@
         <v>0</v>
       </c>
       <c r="N21">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>31</v>
       </c>
@@ -3418,11 +3423,11 @@
         <v>107</v>
       </c>
       <c r="N22">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
@@ -3463,11 +3468,11 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3508,11 +3513,11 @@
         <v>12</v>
       </c>
       <c r="N24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -3553,11 +3558,11 @@
         <v>4</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -3583,7 +3588,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <v>4</v>
@@ -3598,11 +3603,11 @@
         <v>2</v>
       </c>
       <c r="N26">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -3643,11 +3648,11 @@
         <v>0</v>
       </c>
       <c r="N27">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -3688,11 +3693,11 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -3733,11 +3738,11 @@
         <v>1</v>
       </c>
       <c r="N29">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -3751,7 +3756,7 @@
         <v>7</v>
       </c>
       <c r="I30" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -3760,7 +3765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -3774,7 +3779,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -3783,7 +3788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -3806,7 +3811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -3829,7 +3834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -3852,7 +3857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -3875,7 +3880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -3898,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -3921,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -3944,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -3967,7 +3972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="I44" t="s">
         <v>80</v>
       </c>
@@ -3978,11 +3983,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3990,17 +3990,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.59765625" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -4011,7 +4011,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>69</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="5" customFormat="1">
+    <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>78</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>81</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>83</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>85</v>
       </c>
@@ -4071,7 +4071,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>86</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>87</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>88</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>89</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -4131,7 +4131,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>81</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>96</v>
       </c>
@@ -4161,7 +4161,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>90</v>
       </c>
@@ -4172,7 +4172,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>81</v>
       </c>
@@ -4194,12 +4194,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -4210,22 +4210,22 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="5" customFormat="1">
+    <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C23" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C24" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>90</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>31</v>
       </c>
@@ -4247,7 +4247,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>90</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -4269,7 +4269,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>78</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>81</v>
       </c>
@@ -4285,12 +4285,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:4" s="5" customFormat="1">
+    <row r="32" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
         <v>90</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -4326,7 +4326,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C35" s="9" t="s">
         <v>117</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>90</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>90</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C41" s="9" t="s">
         <v>122</v>
       </c>
@@ -4400,7 +4400,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>358</v>
       </c>
@@ -4414,7 +4414,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C43" s="9" t="s">
         <v>507</v>
       </c>
@@ -4422,7 +4422,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>90</v>
       </c>
@@ -4433,17 +4433,17 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="15" t="s">
         <v>209</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>535</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>537</v>
       </c>
@@ -4476,7 +4476,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>114</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>540</v>
       </c>
@@ -4495,7 +4495,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>442</v>
       </c>
@@ -4506,7 +4506,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>76</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="26" thickBot="1">
+    <row r="54" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">
         <v>505</v>
       </c>
@@ -4531,11 +4531,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4543,13 +4538,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="25" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.59765625" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -4569,7 +4564,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1">
+    <row r="2" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>345</v>
       </c>
@@ -4592,7 +4587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="14" customFormat="1">
+    <row r="3" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>358</v>
       </c>
@@ -4615,7 +4610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="14" customFormat="1">
+    <row r="4" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>199</v>
       </c>
@@ -4653,7 +4648,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="14" customFormat="1">
+    <row r="5" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>498</v>
       </c>
@@ -4680,26 +4675,26 @@
       </c>
       <c r="J5" s="5">
         <f>CORREL(C2:C29, Overview!N2:N29)</f>
-        <v>0.43913030963959626</v>
+        <v>0.47331284334556534</v>
       </c>
       <c r="K5" s="14">
         <f>CORREL(D2:D29, Overview!N2:N29)</f>
-        <v>0.47063173876900355</v>
+        <v>0.49821353665145712</v>
       </c>
       <c r="L5" s="14">
         <f>CORREL(E2:E29, Overview!N2:N29)</f>
-        <v>0.56739809209788483</v>
+        <v>0.617563961179595</v>
       </c>
       <c r="M5" s="14">
         <f>CORREL(F2:F29, Overview!N2:N29)</f>
-        <v>0.55191808200486869</v>
+        <v>0.60067998189505989</v>
       </c>
       <c r="N5" s="14">
         <f>CORREL(G2:G29, Overview!N2:N29)</f>
-        <v>0.38403886886909833</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="14" customFormat="1">
+        <v>0.35906066825082744</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>168</v>
       </c>
@@ -4722,7 +4717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="14" customFormat="1">
+    <row r="7" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>400</v>
       </c>
@@ -4745,7 +4740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="14" customFormat="1">
+    <row r="8" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>209</v>
       </c>
@@ -4768,7 +4763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="14" customFormat="1">
+    <row r="9" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>442</v>
       </c>
@@ -4791,7 +4786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="14" customFormat="1">
+    <row r="10" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>391</v>
       </c>
@@ -4814,7 +4809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="17" customFormat="1" ht="26" thickBot="1">
+    <row r="11" spans="1:14" s="17" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>505</v>
       </c>
@@ -4837,7 +4832,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>67</v>
       </c>
@@ -4860,7 +4855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -4883,7 +4878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -4906,7 +4901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -4929,7 +4924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1">
+    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -4952,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -4975,7 +4970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -4998,7 +4993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -5021,7 +5016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -5044,7 +5039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>29</v>
       </c>
@@ -5067,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>31</v>
       </c>
@@ -5090,7 +5085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>33</v>
       </c>
@@ -5113,7 +5108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -5136,7 +5131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -5159,7 +5154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -5182,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -5205,7 +5200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -5228,7 +5223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="20" customFormat="1" ht="26" thickBot="1">
+    <row r="29" spans="1:7" s="20" customFormat="1" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20" t="s">
         <v>45</v>
       </c>
@@ -5251,7 +5246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -5274,7 +5269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -5297,7 +5292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -5320,7 +5315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -5343,7 +5338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -5366,7 +5361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -5389,7 +5384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>59</v>
       </c>
@@ -5412,7 +5407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>61</v>
       </c>
@@ -5435,7 +5430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -5458,7 +5453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -5487,11 +5482,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5504,13 +5494,13 @@
       <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="25" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="5" max="9" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>151</v>
       </c>
@@ -5560,7 +5550,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -5607,7 +5597,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -5654,7 +5644,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -5701,7 +5691,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -5748,7 +5738,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>166</v>
       </c>
@@ -5795,7 +5785,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -5842,7 +5832,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>168</v>
       </c>
@@ -5889,7 +5879,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>169</v>
       </c>
@@ -5936,7 +5926,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>170</v>
       </c>
@@ -5983,7 +5973,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>171</v>
       </c>
@@ -6030,7 +6020,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>172</v>
       </c>
@@ -6077,7 +6067,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>173</v>
       </c>
@@ -6124,7 +6114,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>174</v>
       </c>
@@ -6171,7 +6161,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>175</v>
       </c>
@@ -6218,7 +6208,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>176</v>
       </c>
@@ -6265,7 +6255,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>177</v>
       </c>
@@ -6312,7 +6302,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>178</v>
       </c>
@@ -6359,7 +6349,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>179</v>
       </c>
@@ -6406,7 +6396,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>180</v>
       </c>
@@ -6453,7 +6443,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>181</v>
       </c>
@@ -6500,7 +6490,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>182</v>
       </c>
@@ -6547,7 +6537,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>183</v>
       </c>
@@ -6594,7 +6584,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>184</v>
       </c>
@@ -6641,7 +6631,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>185</v>
       </c>
@@ -6688,7 +6678,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>186</v>
       </c>
@@ -6735,7 +6725,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>187</v>
       </c>
@@ -6782,7 +6772,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>188</v>
       </c>
@@ -6829,7 +6819,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>189</v>
       </c>
@@ -6876,7 +6866,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>190</v>
       </c>
@@ -6923,7 +6913,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>191</v>
       </c>
@@ -6970,7 +6960,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>192</v>
       </c>
@@ -7017,7 +7007,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>193</v>
       </c>
@@ -7064,7 +7054,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>194</v>
       </c>
@@ -7111,7 +7101,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>195</v>
       </c>
@@ -7158,7 +7148,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>196</v>
       </c>
@@ -7205,7 +7195,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>197</v>
       </c>
@@ -7252,7 +7242,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>198</v>
       </c>
@@ -7299,7 +7289,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>199</v>
       </c>
@@ -7346,7 +7336,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>200</v>
       </c>
@@ -7393,7 +7383,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>201</v>
       </c>
@@ -7440,7 +7430,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>202</v>
       </c>
@@ -7487,7 +7477,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>203</v>
       </c>
@@ -7534,7 +7524,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>204</v>
       </c>
@@ -7581,7 +7571,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>205</v>
       </c>
@@ -7628,7 +7618,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>206</v>
       </c>
@@ -7675,7 +7665,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>207</v>
       </c>
@@ -7722,7 +7712,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>208</v>
       </c>
@@ -7769,7 +7759,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>209</v>
       </c>
@@ -7816,7 +7806,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>210</v>
       </c>
@@ -7863,7 +7853,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
         <v>211</v>
       </c>
@@ -7910,7 +7900,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>212</v>
       </c>
@@ -7957,7 +7947,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>213</v>
       </c>
@@ -8004,7 +7994,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>214</v>
       </c>
@@ -8051,7 +8041,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>215</v>
       </c>
@@ -8098,7 +8088,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>216</v>
       </c>
@@ -8145,7 +8135,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>217</v>
       </c>
@@ -8192,7 +8182,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="115" spans="1:15">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>218</v>
       </c>
@@ -8239,7 +8229,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="117" spans="1:15">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>219</v>
       </c>
@@ -8286,7 +8276,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>220</v>
       </c>
@@ -8333,7 +8323,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="121" spans="1:15">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>221</v>
       </c>
@@ -8380,7 +8370,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="123" spans="1:15">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>222</v>
       </c>
@@ -8427,7 +8417,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="125" spans="1:15">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>223</v>
       </c>
@@ -8474,7 +8464,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="127" spans="1:15">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>224</v>
       </c>
@@ -8521,7 +8511,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="129" spans="1:15">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>225</v>
       </c>
@@ -8568,7 +8558,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>226</v>
       </c>
@@ -8615,7 +8605,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>227</v>
       </c>
@@ -8662,7 +8652,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="135" spans="1:15">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>228</v>
       </c>
@@ -8709,7 +8699,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>229</v>
       </c>
@@ -8756,7 +8746,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="139" spans="1:15">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>230</v>
       </c>
@@ -8803,7 +8793,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="141" spans="1:15">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>231</v>
       </c>
@@ -8850,7 +8840,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" s="6" t="s">
         <v>232</v>
       </c>
@@ -8897,7 +8887,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>233</v>
       </c>
@@ -8944,7 +8934,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>234</v>
       </c>
@@ -8991,7 +8981,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>235</v>
       </c>
@@ -9038,7 +9028,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="151" spans="1:15">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>236</v>
       </c>
@@ -9085,7 +9075,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>237</v>
       </c>
@@ -9132,7 +9122,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="155" spans="1:15">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>238</v>
       </c>
@@ -9179,7 +9169,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>239</v>
       </c>
@@ -9226,7 +9216,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="159" spans="1:15">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>240</v>
       </c>
@@ -9273,7 +9263,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>241</v>
       </c>
@@ -9320,7 +9310,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>242</v>
       </c>
@@ -9367,7 +9357,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>243</v>
       </c>
@@ -9414,7 +9404,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>244</v>
       </c>
@@ -9461,7 +9451,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>245</v>
       </c>
@@ -9508,7 +9498,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>246</v>
       </c>
@@ -9555,7 +9545,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="173" spans="1:15">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>247</v>
       </c>
@@ -9602,7 +9592,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="175" spans="1:15">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>248</v>
       </c>
@@ -9649,7 +9639,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="177" spans="1:15">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>249</v>
       </c>
@@ -9696,7 +9686,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="179" spans="1:15">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>250</v>
       </c>
@@ -9743,7 +9733,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="181" spans="1:15">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>251</v>
       </c>
@@ -9790,7 +9780,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="183" spans="1:15">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>252</v>
       </c>
@@ -9837,7 +9827,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="185" spans="1:15">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>253</v>
       </c>
@@ -9884,7 +9874,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="187" spans="1:15">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>254</v>
       </c>
@@ -9931,7 +9921,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="189" spans="1:15">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>255</v>
       </c>
@@ -9978,7 +9968,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="191" spans="1:15">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>256</v>
       </c>
@@ -10025,7 +10015,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="193" spans="1:15">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>257</v>
       </c>
@@ -10072,7 +10062,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="195" spans="1:15">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>258</v>
       </c>
@@ -10119,7 +10109,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="197" spans="1:15">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>259</v>
       </c>
@@ -10166,7 +10156,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="199" spans="1:15">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>260</v>
       </c>
@@ -10213,7 +10203,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="201" spans="1:15">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>261</v>
       </c>
@@ -10260,7 +10250,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="203" spans="1:15">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>262</v>
       </c>
@@ -10307,7 +10297,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="205" spans="1:15">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>263</v>
       </c>
@@ -10354,7 +10344,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="207" spans="1:15">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>264</v>
       </c>
@@ -10401,7 +10391,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="209" spans="1:15">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>265</v>
       </c>
@@ -10448,7 +10438,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="211" spans="1:15">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>266</v>
       </c>
@@ -10495,7 +10485,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="213" spans="1:15">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>267</v>
       </c>
@@ -10542,7 +10532,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="215" spans="1:15">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>268</v>
       </c>
@@ -10589,7 +10579,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="217" spans="1:15">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>269</v>
       </c>
@@ -10636,7 +10626,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="219" spans="1:15">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>270</v>
       </c>
@@ -10683,7 +10673,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="221" spans="1:15">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>271</v>
       </c>
@@ -10730,7 +10720,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="223" spans="1:15">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>272</v>
       </c>
@@ -10777,7 +10767,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="225" spans="1:15">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>273</v>
       </c>
@@ -10824,7 +10814,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="227" spans="1:15">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>274</v>
       </c>
@@ -10871,7 +10861,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="229" spans="1:15">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>275</v>
       </c>
@@ -10918,7 +10908,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="231" spans="1:15">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>276</v>
       </c>
@@ -10965,7 +10955,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="233" spans="1:15">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>277</v>
       </c>
@@ -11012,7 +11002,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="235" spans="1:15">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>278</v>
       </c>
@@ -11059,7 +11049,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="237" spans="1:15">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>279</v>
       </c>
@@ -11106,7 +11096,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="239" spans="1:15">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>280</v>
       </c>
@@ -11153,7 +11143,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="241" spans="1:15">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>281</v>
       </c>
@@ -11200,7 +11190,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="243" spans="1:15">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>282</v>
       </c>
@@ -11247,7 +11237,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="245" spans="1:15">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>283</v>
       </c>
@@ -11294,7 +11284,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="247" spans="1:15">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>284</v>
       </c>
@@ -11341,7 +11331,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="249" spans="1:15">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>285</v>
       </c>
@@ -11388,7 +11378,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="251" spans="1:15">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>286</v>
       </c>
@@ -11435,7 +11425,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="253" spans="1:15">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>287</v>
       </c>
@@ -11482,7 +11472,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="255" spans="1:15">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>288</v>
       </c>
@@ -11529,7 +11519,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="257" spans="1:15">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>289</v>
       </c>
@@ -11576,7 +11566,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="259" spans="1:15">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>290</v>
       </c>
@@ -11623,7 +11613,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="261" spans="1:15">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>291</v>
       </c>
@@ -11670,7 +11660,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="263" spans="1:15">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>292</v>
       </c>
@@ -11717,7 +11707,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="265" spans="1:15">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>293</v>
       </c>
@@ -11764,7 +11754,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="267" spans="1:15">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>294</v>
       </c>
@@ -11811,7 +11801,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="269" spans="1:15">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>295</v>
       </c>
@@ -11858,7 +11848,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="271" spans="1:15">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>296</v>
       </c>
@@ -11905,7 +11895,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="273" spans="1:15">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>297</v>
       </c>
@@ -11952,7 +11942,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="275" spans="1:15">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>298</v>
       </c>
@@ -11999,7 +11989,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="277" spans="1:15">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>299</v>
       </c>
@@ -12046,7 +12036,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="279" spans="1:15">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>300</v>
       </c>
@@ -12093,7 +12083,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="281" spans="1:15">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>301</v>
       </c>
@@ -12140,7 +12130,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="283" spans="1:15">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>302</v>
       </c>
@@ -12187,7 +12177,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="285" spans="1:15">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>303</v>
       </c>
@@ -12234,7 +12224,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="287" spans="1:15">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>304</v>
       </c>
@@ -12281,7 +12271,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="289" spans="1:15">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>305</v>
       </c>
@@ -12328,7 +12318,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="291" spans="1:15">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>306</v>
       </c>
@@ -12375,7 +12365,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="293" spans="1:15">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>307</v>
       </c>
@@ -12422,7 +12412,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="295" spans="1:15">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>308</v>
       </c>
@@ -12469,7 +12459,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="297" spans="1:15">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>309</v>
       </c>
@@ -12516,7 +12506,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="299" spans="1:15">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>310</v>
       </c>
@@ -12563,7 +12553,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="301" spans="1:15">
+    <row r="301" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>311</v>
       </c>
@@ -12610,7 +12600,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="303" spans="1:15">
+    <row r="303" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>312</v>
       </c>
@@ -12657,7 +12647,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="305" spans="1:15">
+    <row r="305" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>313</v>
       </c>
@@ -12704,7 +12694,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="307" spans="1:15">
+    <row r="307" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>314</v>
       </c>
@@ -12751,7 +12741,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="309" spans="1:15">
+    <row r="309" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>315</v>
       </c>
@@ -12798,7 +12788,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="311" spans="1:15">
+    <row r="311" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>316</v>
       </c>
@@ -12845,7 +12835,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="313" spans="1:15">
+    <row r="313" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>317</v>
       </c>
@@ -12892,7 +12882,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="315" spans="1:15">
+    <row r="315" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>318</v>
       </c>
@@ -12939,7 +12929,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="317" spans="1:15">
+    <row r="317" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>319</v>
       </c>
@@ -12986,7 +12976,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="319" spans="1:15">
+    <row r="319" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>320</v>
       </c>
@@ -13033,7 +13023,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="321" spans="1:15">
+    <row r="321" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>321</v>
       </c>
@@ -13080,7 +13070,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="323" spans="1:15">
+    <row r="323" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>322</v>
       </c>
@@ -13127,7 +13117,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="325" spans="1:15">
+    <row r="325" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>323</v>
       </c>
@@ -13174,7 +13164,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="327" spans="1:15">
+    <row r="327" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>324</v>
       </c>
@@ -13221,7 +13211,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="329" spans="1:15">
+    <row r="329" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A329" s="6" t="s">
         <v>325</v>
       </c>
@@ -13268,7 +13258,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="331" spans="1:15">
+    <row r="331" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>326</v>
       </c>
@@ -13315,7 +13305,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="333" spans="1:15">
+    <row r="333" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>327</v>
       </c>
@@ -13362,7 +13352,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="335" spans="1:15">
+    <row r="335" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>328</v>
       </c>
@@ -13409,7 +13399,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="337" spans="1:15">
+    <row r="337" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A337" t="s">
         <v>329</v>
       </c>
@@ -13456,7 +13446,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="339" spans="1:15">
+    <row r="339" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A339" t="s">
         <v>330</v>
       </c>
@@ -13503,7 +13493,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="341" spans="1:15">
+    <row r="341" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A341" t="s">
         <v>331</v>
       </c>
@@ -13550,7 +13540,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="343" spans="1:15">
+    <row r="343" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A343" t="s">
         <v>332</v>
       </c>
@@ -13597,7 +13587,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="345" spans="1:15">
+    <row r="345" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
         <v>333</v>
       </c>
@@ -13644,7 +13634,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="347" spans="1:15">
+    <row r="347" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
         <v>334</v>
       </c>
@@ -13691,7 +13681,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="349" spans="1:15">
+    <row r="349" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A349" t="s">
         <v>335</v>
       </c>
@@ -13738,7 +13728,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="351" spans="1:15">
+    <row r="351" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A351" t="s">
         <v>336</v>
       </c>
@@ -13785,7 +13775,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="353" spans="1:15">
+    <row r="353" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A353" t="s">
         <v>337</v>
       </c>
@@ -13832,7 +13822,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="355" spans="1:15">
+    <row r="355" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
         <v>338</v>
       </c>
@@ -13879,7 +13869,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="357" spans="1:15">
+    <row r="357" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A357" t="s">
         <v>339</v>
       </c>
@@ -13926,7 +13916,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="359" spans="1:15">
+    <row r="359" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A359" t="s">
         <v>340</v>
       </c>
@@ -13973,7 +13963,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="361" spans="1:15">
+    <row r="361" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A361" t="s">
         <v>341</v>
       </c>
@@ -14020,7 +14010,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="363" spans="1:15">
+    <row r="363" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A363" t="s">
         <v>342</v>
       </c>
@@ -14067,7 +14057,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="365" spans="1:15">
+    <row r="365" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A365" t="s">
         <v>343</v>
       </c>
@@ -14114,7 +14104,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="367" spans="1:15">
+    <row r="367" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A367" t="s">
         <v>344</v>
       </c>
@@ -14161,7 +14151,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="369" spans="1:15">
+    <row r="369" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A369" t="s">
         <v>345</v>
       </c>
@@ -14208,7 +14198,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="371" spans="1:15">
+    <row r="371" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A371" t="s">
         <v>346</v>
       </c>
@@ -14255,7 +14245,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="373" spans="1:15">
+    <row r="373" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A373" t="s">
         <v>347</v>
       </c>
@@ -14302,7 +14292,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="375" spans="1:15">
+    <row r="375" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
         <v>348</v>
       </c>
@@ -14349,7 +14339,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="377" spans="1:15">
+    <row r="377" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A377" t="s">
         <v>349</v>
       </c>
@@ -14396,7 +14386,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="379" spans="1:15">
+    <row r="379" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A379" t="s">
         <v>350</v>
       </c>
@@ -14443,7 +14433,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="381" spans="1:15">
+    <row r="381" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A381" t="s">
         <v>351</v>
       </c>
@@ -14490,7 +14480,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="383" spans="1:15">
+    <row r="383" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A383" t="s">
         <v>352</v>
       </c>
@@ -14537,7 +14527,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="385" spans="1:15">
+    <row r="385" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A385" t="s">
         <v>353</v>
       </c>
@@ -14584,7 +14574,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="387" spans="1:15">
+    <row r="387" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A387" t="s">
         <v>354</v>
       </c>
@@ -14631,7 +14621,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="389" spans="1:15">
+    <row r="389" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
         <v>355</v>
       </c>
@@ -14678,7 +14668,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="391" spans="1:15">
+    <row r="391" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A391" t="s">
         <v>356</v>
       </c>
@@ -14725,7 +14715,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="393" spans="1:15">
+    <row r="393" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A393" t="s">
         <v>357</v>
       </c>
@@ -14772,7 +14762,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="395" spans="1:15">
+    <row r="395" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A395" t="s">
         <v>358</v>
       </c>
@@ -14819,7 +14809,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="397" spans="1:15">
+    <row r="397" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A397" t="s">
         <v>359</v>
       </c>
@@ -14866,7 +14856,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="399" spans="1:15">
+    <row r="399" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A399" t="s">
         <v>360</v>
       </c>
@@ -14913,7 +14903,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="401" spans="1:15">
+    <row r="401" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A401" t="s">
         <v>361</v>
       </c>
@@ -14960,7 +14950,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="403" spans="1:15">
+    <row r="403" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A403" t="s">
         <v>362</v>
       </c>
@@ -15007,7 +14997,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="405" spans="1:15">
+    <row r="405" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A405" t="s">
         <v>363</v>
       </c>
@@ -15054,7 +15044,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="407" spans="1:15">
+    <row r="407" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A407" t="s">
         <v>364</v>
       </c>
@@ -15101,7 +15091,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="409" spans="1:15">
+    <row r="409" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
         <v>365</v>
       </c>
@@ -15148,7 +15138,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="411" spans="1:15">
+    <row r="411" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A411" t="s">
         <v>366</v>
       </c>
@@ -15195,7 +15185,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="413" spans="1:15">
+    <row r="413" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A413" t="s">
         <v>367</v>
       </c>
@@ -15242,7 +15232,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="415" spans="1:15">
+    <row r="415" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A415" s="6" t="s">
         <v>368</v>
       </c>
@@ -15289,7 +15279,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="417" spans="1:15">
+    <row r="417" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A417" t="s">
         <v>369</v>
       </c>
@@ -15336,7 +15326,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="419" spans="1:15">
+    <row r="419" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A419" t="s">
         <v>370</v>
       </c>
@@ -15383,7 +15373,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="421" spans="1:15">
+    <row r="421" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A421" t="s">
         <v>371</v>
       </c>
@@ -15430,7 +15420,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="423" spans="1:15">
+    <row r="423" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
         <v>372</v>
       </c>
@@ -15477,7 +15467,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="425" spans="1:15">
+    <row r="425" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A425" t="s">
         <v>373</v>
       </c>
@@ -15524,7 +15514,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="427" spans="1:15">
+    <row r="427" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A427" t="s">
         <v>374</v>
       </c>
@@ -15571,7 +15561,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="429" spans="1:15">
+    <row r="429" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A429" t="s">
         <v>375</v>
       </c>
@@ -15618,7 +15608,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="431" spans="1:15">
+    <row r="431" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A431" t="s">
         <v>376</v>
       </c>
@@ -15665,7 +15655,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="433" spans="1:15">
+    <row r="433" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
         <v>377</v>
       </c>
@@ -15712,7 +15702,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="435" spans="1:15">
+    <row r="435" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A435" t="s">
         <v>378</v>
       </c>
@@ -15759,7 +15749,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="437" spans="1:15">
+    <row r="437" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A437" t="s">
         <v>379</v>
       </c>
@@ -15806,7 +15796,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="439" spans="1:15">
+    <row r="439" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A439" t="s">
         <v>380</v>
       </c>
@@ -15853,7 +15843,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="441" spans="1:15">
+    <row r="441" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A441" t="s">
         <v>381</v>
       </c>
@@ -15900,7 +15890,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="443" spans="1:15">
+    <row r="443" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A443" t="s">
         <v>382</v>
       </c>
@@ -15947,7 +15937,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="445" spans="1:15">
+    <row r="445" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A445" t="s">
         <v>383</v>
       </c>
@@ -15994,7 +15984,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="447" spans="1:15">
+    <row r="447" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A447" t="s">
         <v>384</v>
       </c>
@@ -16041,7 +16031,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="449" spans="1:15">
+    <row r="449" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A449" t="s">
         <v>385</v>
       </c>
@@ -16088,7 +16078,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="451" spans="1:15">
+    <row r="451" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A451" t="s">
         <v>386</v>
       </c>
@@ -16135,7 +16125,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="453" spans="1:15">
+    <row r="453" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
         <v>387</v>
       </c>
@@ -16182,7 +16172,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="455" spans="1:15">
+    <row r="455" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A455" t="s">
         <v>388</v>
       </c>
@@ -16229,7 +16219,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="457" spans="1:15">
+    <row r="457" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A457" s="6" t="s">
         <v>389</v>
       </c>
@@ -16276,7 +16266,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="459" spans="1:15">
+    <row r="459" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A459" t="s">
         <v>390</v>
       </c>
@@ -16323,7 +16313,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="461" spans="1:15">
+    <row r="461" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A461" t="s">
         <v>391</v>
       </c>
@@ -16370,7 +16360,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="463" spans="1:15">
+    <row r="463" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A463" t="s">
         <v>392</v>
       </c>
@@ -16417,7 +16407,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="465" spans="1:15">
+    <row r="465" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A465" t="s">
         <v>393</v>
       </c>
@@ -16464,7 +16454,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="467" spans="1:15">
+    <row r="467" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A467" t="s">
         <v>394</v>
       </c>
@@ -16511,7 +16501,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="469" spans="1:15">
+    <row r="469" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A469" t="s">
         <v>395</v>
       </c>
@@ -16558,7 +16548,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="471" spans="1:15">
+    <row r="471" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A471" t="s">
         <v>396</v>
       </c>
@@ -16605,7 +16595,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="473" spans="1:15">
+    <row r="473" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
         <v>397</v>
       </c>
@@ -16652,7 +16642,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="475" spans="1:15">
+    <row r="475" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A475" t="s">
         <v>398</v>
       </c>
@@ -16699,7 +16689,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="477" spans="1:15">
+    <row r="477" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A477" t="s">
         <v>399</v>
       </c>
@@ -16746,7 +16736,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="479" spans="1:15">
+    <row r="479" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A479" s="6" t="s">
         <v>400</v>
       </c>
@@ -16793,7 +16783,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="481" spans="1:15">
+    <row r="481" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A481" t="s">
         <v>401</v>
       </c>
@@ -16840,7 +16830,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="483" spans="1:15">
+    <row r="483" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A483" t="s">
         <v>402</v>
       </c>
@@ -16887,7 +16877,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="485" spans="1:15">
+    <row r="485" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A485" t="s">
         <v>403</v>
       </c>
@@ -16934,7 +16924,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="487" spans="1:15">
+    <row r="487" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A487" t="s">
         <v>404</v>
       </c>
@@ -16981,7 +16971,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="489" spans="1:15">
+    <row r="489" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A489" t="s">
         <v>405</v>
       </c>
@@ -17028,7 +17018,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="491" spans="1:15">
+    <row r="491" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>406</v>
       </c>
@@ -17075,7 +17065,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="493" spans="1:15">
+    <row r="493" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>407</v>
       </c>
@@ -17122,7 +17112,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="495" spans="1:15">
+    <row r="495" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>408</v>
       </c>
@@ -17169,7 +17159,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="497" spans="1:15">
+    <row r="497" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>409</v>
       </c>
@@ -17216,7 +17206,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="499" spans="1:15">
+    <row r="499" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>410</v>
       </c>
@@ -17263,7 +17253,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="501" spans="1:15">
+    <row r="501" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>411</v>
       </c>
@@ -17310,7 +17300,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="503" spans="1:15">
+    <row r="503" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>412</v>
       </c>
@@ -17357,7 +17347,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="505" spans="1:15">
+    <row r="505" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>413</v>
       </c>
@@ -17404,7 +17394,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="507" spans="1:15">
+    <row r="507" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>414</v>
       </c>
@@ -17451,7 +17441,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="509" spans="1:15">
+    <row r="509" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>415</v>
       </c>
@@ -17498,7 +17488,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="511" spans="1:15">
+    <row r="511" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>416</v>
       </c>
@@ -17545,7 +17535,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="513" spans="1:15">
+    <row r="513" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>417</v>
       </c>
@@ -17592,7 +17582,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="515" spans="1:15">
+    <row r="515" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>418</v>
       </c>
@@ -17639,7 +17629,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="517" spans="1:15">
+    <row r="517" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
         <v>419</v>
       </c>
@@ -17686,7 +17676,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="519" spans="1:15">
+    <row r="519" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A519" t="s">
         <v>420</v>
       </c>
@@ -17733,7 +17723,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="521" spans="1:15">
+    <row r="521" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A521" t="s">
         <v>421</v>
       </c>
@@ -17780,7 +17770,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="523" spans="1:15">
+    <row r="523" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A523" t="s">
         <v>422</v>
       </c>
@@ -17827,7 +17817,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="525" spans="1:15">
+    <row r="525" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A525" t="s">
         <v>423</v>
       </c>
@@ -17874,7 +17864,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="527" spans="1:15">
+    <row r="527" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A527" t="s">
         <v>424</v>
       </c>
@@ -17921,7 +17911,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="529" spans="1:15">
+    <row r="529" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A529" t="s">
         <v>425</v>
       </c>
@@ -17968,7 +17958,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="531" spans="1:15">
+    <row r="531" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A531" t="s">
         <v>426</v>
       </c>
@@ -18015,7 +18005,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="533" spans="1:15">
+    <row r="533" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A533" t="s">
         <v>427</v>
       </c>
@@ -18062,7 +18052,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="535" spans="1:15">
+    <row r="535" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A535" t="s">
         <v>428</v>
       </c>
@@ -18109,7 +18099,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="537" spans="1:15">
+    <row r="537" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A537" t="s">
         <v>429</v>
       </c>
@@ -18156,7 +18146,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="539" spans="1:15">
+    <row r="539" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A539" t="s">
         <v>430</v>
       </c>
@@ -18203,7 +18193,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="541" spans="1:15">
+    <row r="541" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A541" t="s">
         <v>431</v>
       </c>
@@ -18250,7 +18240,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="543" spans="1:15">
+    <row r="543" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A543" t="s">
         <v>432</v>
       </c>
@@ -18297,7 +18287,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="545" spans="1:15">
+    <row r="545" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A545" t="s">
         <v>433</v>
       </c>
@@ -18344,7 +18334,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="547" spans="1:15">
+    <row r="547" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A547" t="s">
         <v>434</v>
       </c>
@@ -18391,7 +18381,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="549" spans="1:15">
+    <row r="549" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A549" t="s">
         <v>435</v>
       </c>
@@ -18438,7 +18428,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="551" spans="1:15">
+    <row r="551" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A551" t="s">
         <v>436</v>
       </c>
@@ -18485,7 +18475,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="553" spans="1:15">
+    <row r="553" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A553" t="s">
         <v>437</v>
       </c>
@@ -18532,7 +18522,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="555" spans="1:15">
+    <row r="555" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A555" t="s">
         <v>438</v>
       </c>
@@ -18579,7 +18569,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="557" spans="1:15">
+    <row r="557" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A557" t="s">
         <v>439</v>
       </c>
@@ -18626,7 +18616,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="559" spans="1:15">
+    <row r="559" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A559" t="s">
         <v>440</v>
       </c>
@@ -18673,7 +18663,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="561" spans="1:15">
+    <row r="561" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A561" t="s">
         <v>441</v>
       </c>
@@ -18720,7 +18710,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="563" spans="1:15">
+    <row r="563" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A563" t="s">
         <v>442</v>
       </c>
@@ -18767,7 +18757,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="565" spans="1:15">
+    <row r="565" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A565" t="s">
         <v>443</v>
       </c>
@@ -18814,7 +18804,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="567" spans="1:15">
+    <row r="567" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A567" t="s">
         <v>444</v>
       </c>
@@ -18861,7 +18851,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="569" spans="1:15">
+    <row r="569" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A569" t="s">
         <v>445</v>
       </c>
@@ -18908,7 +18898,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="571" spans="1:15">
+    <row r="571" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A571" t="s">
         <v>446</v>
       </c>
@@ -18955,7 +18945,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="573" spans="1:15">
+    <row r="573" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A573" t="s">
         <v>447</v>
       </c>
@@ -19002,7 +18992,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="575" spans="1:15">
+    <row r="575" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A575" t="s">
         <v>448</v>
       </c>
@@ -19049,7 +19039,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="577" spans="1:15">
+    <row r="577" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A577" t="s">
         <v>449</v>
       </c>
@@ -19096,7 +19086,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="579" spans="1:15">
+    <row r="579" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A579" t="s">
         <v>450</v>
       </c>
@@ -19143,7 +19133,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="581" spans="1:15">
+    <row r="581" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A581" t="s">
         <v>451</v>
       </c>
@@ -19190,7 +19180,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="583" spans="1:15">
+    <row r="583" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A583" t="s">
         <v>452</v>
       </c>
@@ -19237,7 +19227,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="585" spans="1:15">
+    <row r="585" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A585" t="s">
         <v>453</v>
       </c>
@@ -19284,7 +19274,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="587" spans="1:15">
+    <row r="587" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A587" t="s">
         <v>454</v>
       </c>
@@ -19331,7 +19321,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="589" spans="1:15">
+    <row r="589" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A589" t="s">
         <v>455</v>
       </c>
@@ -19378,7 +19368,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="591" spans="1:15">
+    <row r="591" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A591" t="s">
         <v>456</v>
       </c>
@@ -19425,7 +19415,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="593" spans="1:15">
+    <row r="593" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A593" t="s">
         <v>457</v>
       </c>
@@ -19472,7 +19462,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="595" spans="1:15">
+    <row r="595" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A595" t="s">
         <v>458</v>
       </c>
@@ -19519,7 +19509,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="597" spans="1:15">
+    <row r="597" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A597" t="s">
         <v>459</v>
       </c>
@@ -19566,7 +19556,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="599" spans="1:15">
+    <row r="599" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A599" t="s">
         <v>460</v>
       </c>
@@ -19613,7 +19603,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="601" spans="1:15">
+    <row r="601" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A601" t="s">
         <v>461</v>
       </c>
@@ -19660,7 +19650,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="603" spans="1:15">
+    <row r="603" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A603" t="s">
         <v>462</v>
       </c>
@@ -19707,7 +19697,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="605" spans="1:15">
+    <row r="605" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A605" t="s">
         <v>463</v>
       </c>
@@ -19754,7 +19744,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="607" spans="1:15">
+    <row r="607" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A607" t="s">
         <v>464</v>
       </c>
@@ -19801,7 +19791,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="609" spans="1:15">
+    <row r="609" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A609" t="s">
         <v>465</v>
       </c>
@@ -19848,7 +19838,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="611" spans="1:15">
+    <row r="611" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A611" t="s">
         <v>466</v>
       </c>
@@ -19895,7 +19885,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="613" spans="1:15">
+    <row r="613" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A613" t="s">
         <v>467</v>
       </c>
@@ -19942,7 +19932,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="615" spans="1:15">
+    <row r="615" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A615" t="s">
         <v>468</v>
       </c>
@@ -19989,7 +19979,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="617" spans="1:15">
+    <row r="617" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A617" t="s">
         <v>469</v>
       </c>
@@ -20036,7 +20026,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="619" spans="1:15">
+    <row r="619" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A619" t="s">
         <v>470</v>
       </c>
@@ -20083,7 +20073,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="621" spans="1:15">
+    <row r="621" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A621" t="s">
         <v>471</v>
       </c>
@@ -20130,7 +20120,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="623" spans="1:15">
+    <row r="623" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A623" t="s">
         <v>472</v>
       </c>
@@ -20177,7 +20167,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="625" spans="1:15">
+    <row r="625" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A625" t="s">
         <v>473</v>
       </c>
@@ -20224,7 +20214,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="627" spans="1:15">
+    <row r="627" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A627" t="s">
         <v>474</v>
       </c>
@@ -20271,7 +20261,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="629" spans="1:15">
+    <row r="629" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A629" t="s">
         <v>475</v>
       </c>
@@ -20318,7 +20308,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="631" spans="1:15">
+    <row r="631" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A631" t="s">
         <v>476</v>
       </c>
@@ -20365,7 +20355,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="633" spans="1:15">
+    <row r="633" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A633" t="s">
         <v>477</v>
       </c>
@@ -20412,7 +20402,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="635" spans="1:15">
+    <row r="635" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A635" t="s">
         <v>478</v>
       </c>
@@ -20459,7 +20449,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="637" spans="1:15">
+    <row r="637" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A637" t="s">
         <v>479</v>
       </c>
@@ -20506,7 +20496,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="639" spans="1:15">
+    <row r="639" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A639" t="s">
         <v>480</v>
       </c>
@@ -20553,7 +20543,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="641" spans="1:15">
+    <row r="641" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A641" t="s">
         <v>481</v>
       </c>
@@ -20600,7 +20590,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="643" spans="1:15">
+    <row r="643" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A643" t="s">
         <v>482</v>
       </c>
@@ -20647,7 +20637,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="645" spans="1:15">
+    <row r="645" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A645" s="6" t="s">
         <v>483</v>
       </c>
@@ -20694,7 +20684,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="647" spans="1:15">
+    <row r="647" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A647" t="s">
         <v>484</v>
       </c>
@@ -20741,7 +20731,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="649" spans="1:15">
+    <row r="649" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A649" t="s">
         <v>485</v>
       </c>
@@ -20788,7 +20778,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="651" spans="1:15">
+    <row r="651" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A651" t="s">
         <v>486</v>
       </c>
@@ -20835,7 +20825,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="653" spans="1:15">
+    <row r="653" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A653" t="s">
         <v>487</v>
       </c>
@@ -20882,7 +20872,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="655" spans="1:15">
+    <row r="655" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A655" t="s">
         <v>488</v>
       </c>
@@ -20929,7 +20919,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="657" spans="1:15">
+    <row r="657" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A657" t="s">
         <v>489</v>
       </c>
@@ -20976,7 +20966,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="659" spans="1:15">
+    <row r="659" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A659" t="s">
         <v>490</v>
       </c>
@@ -21023,7 +21013,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="661" spans="1:15">
+    <row r="661" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A661" t="s">
         <v>491</v>
       </c>
@@ -21070,7 +21060,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="663" spans="1:15">
+    <row r="663" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A663" t="s">
         <v>492</v>
       </c>
@@ -21117,7 +21107,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="665" spans="1:15">
+    <row r="665" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A665" t="s">
         <v>493</v>
       </c>
@@ -21164,7 +21154,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="667" spans="1:15">
+    <row r="667" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A667" t="s">
         <v>494</v>
       </c>
@@ -21211,7 +21201,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="669" spans="1:15">
+    <row r="669" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A669" t="s">
         <v>495</v>
       </c>
@@ -21258,7 +21248,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="671" spans="1:15">
+    <row r="671" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A671" t="s">
         <v>496</v>
       </c>
@@ -21305,7 +21295,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="673" spans="1:15">
+    <row r="673" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A673" t="s">
         <v>497</v>
       </c>
@@ -21352,7 +21342,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="675" spans="1:15">
+    <row r="675" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A675" t="s">
         <v>498</v>
       </c>
@@ -21399,7 +21389,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="677" spans="1:15">
+    <row r="677" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A677" t="s">
         <v>499</v>
       </c>
@@ -21446,7 +21436,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="679" spans="1:15">
+    <row r="679" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A679" t="s">
         <v>500</v>
       </c>
@@ -21493,7 +21483,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="681" spans="1:15">
+    <row r="681" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A681" t="s">
         <v>501</v>
       </c>
@@ -21540,7 +21530,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="683" spans="1:15">
+    <row r="683" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A683" t="s">
         <v>502</v>
       </c>
@@ -21587,7 +21577,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="685" spans="1:15">
+    <row r="685" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A685" t="s">
         <v>503</v>
       </c>
@@ -21634,7 +21624,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="687" spans="1:15">
+    <row r="687" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A687" t="s">
         <v>504</v>
       </c>
@@ -21683,10 +21673,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
big edits, only 1 column over
</commit_message>
<xml_diff>
--- a/kodu_programs.xlsx
+++ b/kodu_programs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="16580" windowHeight="14820" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="22860" windowHeight="23580"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -2220,8 +2220,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG44"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="82" zoomScaleNormal="82" zoomScalePageLayoutView="82" workbookViewId="0">
+      <selection activeCell="D16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.59765625" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -2407,7 +2407,7 @@
         <v>2</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N2:N12" si="0">COUNTIF(D3:M3, "&gt;0")</f>
+        <f t="shared" ref="N3:N12" si="0">COUNTIF(D3:M3, "&gt;0")</f>
         <v>4</v>
       </c>
       <c r="O3" s="2" t="s">
@@ -2738,7 +2738,7 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2">
         <f>AVERAGE(N12:N29)</f>
-        <v>2.2777777777777777</v>
+        <v>2.4117647058823528</v>
       </c>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -3130,32 +3130,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:33" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" ht="26" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="I16" s="7">
-        <v>0</v>
-      </c>
-      <c r="J16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -3787,6 +3769,10 @@
       <c r="L31">
         <v>0</v>
       </c>
+      <c r="N31">
+        <f>COUNTA(N2:N29)</f>
+        <v>27</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -3810,6 +3796,10 @@
       <c r="L32">
         <v>0</v>
       </c>
+      <c r="N32">
+        <f>COUNTIF(N2:N29, "&gt;0")</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
@@ -3970,6 +3960,24 @@
       </c>
       <c r="L39">
         <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G41">
+        <f>COUNTA(G2:G29)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <f>COUNTIF(G2:G29, "&gt;0")</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G43">
+        <f>G42/G41</f>
+        <v>0.81481481481481477</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -4538,7 +4546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -4675,23 +4683,23 @@
       </c>
       <c r="J5" s="5">
         <f>CORREL(C2:C29, Overview!N2:N29)</f>
-        <v>0.47331284334556534</v>
+        <v>0.43313216729628767</v>
       </c>
       <c r="K5" s="14">
         <f>CORREL(D2:D29, Overview!N2:N29)</f>
-        <v>0.49821353665145712</v>
+        <v>0.47046765202150648</v>
       </c>
       <c r="L5" s="14">
         <f>CORREL(E2:E29, Overview!N2:N29)</f>
-        <v>0.617563961179595</v>
+        <v>0.60324827094402256</v>
       </c>
       <c r="M5" s="14">
         <f>CORREL(F2:F29, Overview!N2:N29)</f>
-        <v>0.60067998189505989</v>
+        <v>0.58484837608893936</v>
       </c>
       <c r="N5" s="14">
         <f>CORREL(G2:G29, Overview!N2:N29)</f>
-        <v>0.35906066825082744</v>
+        <v>0.35458897737603634</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>